<commit_message>
add component and package.json
</commit_message>
<xml_diff>
--- a/docs/gannt chart.xlsx
+++ b/docs/gannt chart.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Item</t>
   </si>
@@ -99,14 +99,49 @@
   </si>
   <si>
     <t>edits</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>interviews (tak, kevin, Ric)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -137,8 +172,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,8 +236,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -202,31 +275,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -234,12 +332,39 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -515,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -592,141 +717,194 @@
         <v>43126</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:20" s="15" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="R3" s="12"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="12"/>
+      <c r="P4" s="17"/>
+      <c r="R4" s="12"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C8" s="9"/>
       <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>4</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C9" s="9"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E13" s="9"/>
       <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="10"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="I14" s="10"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="9"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="9"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="9"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="10"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="10"/>
@@ -735,23 +913,23 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="9"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>16</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I22" s="10"/>
       <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -760,24 +938,42 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
       <c r="M24" s="9"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="M25" s="9"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="9"/>
       <c r="P25" s="10"/>
       <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
     </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+    </row>
+    <row r="27" spans="1:18" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
profile create from db
</commit_message>
<xml_diff>
--- a/docs/gannt chart.xlsx
+++ b/docs/gannt chart.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
-  <workbookPr/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/riclavers/site/w_23/musicACT/docs/"/>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$T$27</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -132,7 +135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +203,12 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -640,10 +649,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -805,14 +817,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -825,7 +837,7 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -973,7 +985,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="8" scale="76" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>